<commit_message>
To imporve and test the KnownLenses in ml code
</commit_message>
<xml_diff>
--- a/Results /17 April 2020.xlsx
+++ b/Results /17 April 2020.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annarienbester/git/gravitationallenses/Results /"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72D0F908-BDA8-0D49-9ED2-317468553BE3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C593C775-6F43-FF40-863F-40429BAA0C4D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{EE8A5D69-8514-D648-BD1F-175D6DB078D3}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{EE8A5D69-8514-D648-BD1F-175D6DB078D3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="76">
   <si>
     <t>Negative DES</t>
   </si>
@@ -225,13 +225,49 @@
   </si>
   <si>
     <t>241/256</t>
+  </si>
+  <si>
+    <t>X = Images</t>
+  </si>
+  <si>
+    <t>Y = Labels</t>
+  </si>
+  <si>
+    <t>Accuracy Rate</t>
+  </si>
+  <si>
+    <t>0.965</t>
+  </si>
+  <si>
+    <t>clf_image = MLPClassifier(activation = 'relu',</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hidden_layer_sizes = (100, 100, 100), </t>
+  </si>
+  <si>
+    <t xml:space="preserve">solver='adam', </t>
+  </si>
+  <si>
+    <t>verbose=True,</t>
+  </si>
+  <si>
+    <t>max_iter=100)</t>
+  </si>
+  <si>
+    <t>Test on DES2017</t>
+  </si>
+  <si>
+    <t>Test on Jacobs</t>
+  </si>
+  <si>
+    <t>Test on DES2017+Jacobs</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -246,6 +282,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -255,7 +297,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -456,32 +498,94 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
@@ -491,6 +595,33 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -805,109 +936,109 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A06CD785-33B7-3045-A313-C2EB4D15E3B6}">
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.83203125" customWidth="1"/>
+    <col min="1" max="1" width="22.33203125" customWidth="1"/>
     <col min="2" max="2" width="24.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="41.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="56.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="35.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="5" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8"/>
-      <c r="B2" s="12" t="s">
+      <c r="A2" s="13"/>
+      <c r="B2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="6"/>
-      <c r="B4" s="15" t="s">
+      <c r="A4" s="14"/>
+      <c r="B4" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="D4" s="10" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
-      <c r="B5" s="12" t="s">
+      <c r="A5" s="15"/>
+      <c r="B5" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D5" s="8" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="17"/>
-      <c r="B6" s="17"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
+      <c r="A6" s="11"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="17"/>
-      <c r="B7" s="17"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
+      <c r="A7" s="11"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="1" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="2"/>
+      <c r="A9" s="16"/>
       <c r="B9" t="s">
         <v>26</v>
       </c>
@@ -916,7 +1047,7 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="2"/>
+      <c r="A10" s="16"/>
       <c r="B10" t="s">
         <v>27</v>
       </c>
@@ -925,7 +1056,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="2"/>
+      <c r="A11" s="16"/>
       <c r="B11" t="s">
         <v>28</v>
       </c>
@@ -934,7 +1065,7 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="2"/>
+      <c r="A12" s="16"/>
       <c r="B12" t="s">
         <v>29</v>
       </c>
@@ -943,7 +1074,7 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="2"/>
+      <c r="A13" s="16"/>
       <c r="B13" t="s">
         <v>22</v>
       </c>
@@ -952,7 +1083,7 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="2"/>
+      <c r="A14" s="16"/>
       <c r="B14" t="s">
         <v>25</v>
       </c>
@@ -961,7 +1092,7 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="2"/>
+      <c r="A15" s="16"/>
       <c r="B15" t="s">
         <v>31</v>
       </c>
@@ -970,7 +1101,7 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="2"/>
+      <c r="A16" s="16"/>
       <c r="B16" t="s">
         <v>34</v>
       </c>
@@ -979,7 +1110,7 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="2"/>
+      <c r="A17" s="16"/>
       <c r="B17" t="s">
         <v>36</v>
       </c>
@@ -988,7 +1119,7 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="2"/>
+      <c r="A18" s="16"/>
       <c r="B18" t="s">
         <v>38</v>
       </c>
@@ -997,7 +1128,7 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="2"/>
+      <c r="A19" s="16"/>
       <c r="B19" t="s">
         <v>40</v>
       </c>
@@ -1006,7 +1137,7 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="2"/>
+      <c r="A20" s="16"/>
       <c r="B20" t="s">
         <v>42</v>
       </c>
@@ -1015,7 +1146,7 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="2"/>
+      <c r="A21" s="16"/>
       <c r="B21" t="s">
         <v>44</v>
       </c>
@@ -1024,13 +1155,13 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="2"/>
+      <c r="A22" s="16"/>
     </row>
     <row r="23" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
+      <c r="A23" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="B23" s="1"/>
+      <c r="B23" s="17"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
@@ -1161,6 +1292,76 @@
         <f>(241/256)*100</f>
         <v>94.140625</v>
       </c>
+    </row>
+    <row r="33" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="B34" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="C34" s="20" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="B35" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="C35" s="22" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" s="21"/>
+      <c r="B36" s="11"/>
+      <c r="C36" s="22" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" s="21"/>
+      <c r="B37" s="11"/>
+      <c r="C37" s="22" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" s="21"/>
+      <c r="B38" s="11"/>
+      <c r="C38" s="22" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" s="21"/>
+      <c r="B39" s="11"/>
+      <c r="C39" s="23"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="B40" s="11"/>
+      <c r="C40" s="23"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="B41" s="11"/>
+      <c r="C41" s="23"/>
+    </row>
+    <row r="42" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="B42" s="25"/>
+      <c r="C42" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
Some changes to path names
</commit_message>
<xml_diff>
--- a/Results /17 April 2020.xlsx
+++ b/Results /17 April 2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annarienbester/git/gravitationallenses/Results /"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9994BE22-1245-464F-B487-94D0DAD93F55}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC1EF340-A24F-3F4F-87E5-671BEDD52D09}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{EE8A5D69-8514-D648-BD1F-175D6DB078D3}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Negative DES</t>
   </si>
@@ -86,159 +86,6 @@
     <t>KnownLenses/Jacobs_KnownLenses/num_source/</t>
   </si>
   <si>
-    <t>Using _norm.fits</t>
-  </si>
-  <si>
-    <t>0.9999</t>
-  </si>
-  <si>
-    <t>1.0005</t>
-  </si>
-  <si>
-    <t>1.0003</t>
-  </si>
-  <si>
-    <t>0.0002</t>
-  </si>
-  <si>
-    <t>DES2017.std</t>
-  </si>
-  <si>
-    <t>Data Check</t>
-  </si>
-  <si>
-    <t>Standard Deviation/ Mean</t>
-  </si>
-  <si>
-    <t>Unknown(47).mean</t>
-  </si>
-  <si>
-    <t>DataPos.std</t>
-  </si>
-  <si>
-    <t>DataNeg.std</t>
-  </si>
-  <si>
-    <t>AllData.std</t>
-  </si>
-  <si>
-    <t>DES2017.mean</t>
-  </si>
-  <si>
-    <t>0.0005</t>
-  </si>
-  <si>
-    <t>Unknown(47).std</t>
-  </si>
-  <si>
-    <t>1.0011</t>
-  </si>
-  <si>
-    <t>Jacobs</t>
-  </si>
-  <si>
-    <t>Jacobs(84).mean</t>
-  </si>
-  <si>
-    <t>0.0000</t>
-  </si>
-  <si>
-    <t>Jacobs(84).std</t>
-  </si>
-  <si>
-    <t>1.0000</t>
-  </si>
-  <si>
-    <t>DES2017+Jacobs(131).mean</t>
-  </si>
-  <si>
-    <t>2.310732</t>
-  </si>
-  <si>
-    <t>DES2017+Jacobs(131).std</t>
-  </si>
-  <si>
-    <t>77.5805</t>
-  </si>
-  <si>
-    <t>Unknown(256).mean</t>
-  </si>
-  <si>
-    <t>4.1911</t>
-  </si>
-  <si>
-    <t>Unknown(256).std</t>
-  </si>
-  <si>
-    <t>89.3141</t>
-  </si>
-  <si>
-    <t>where #1 = lenses, #0 = nonlenses</t>
-  </si>
-  <si>
-    <t>UNSEEN</t>
-  </si>
-  <si>
-    <t>DATA</t>
-  </si>
-  <si>
-    <t>#1</t>
-  </si>
-  <si>
-    <t>#0</t>
-  </si>
-  <si>
-    <t>FRACTIONS</t>
-  </si>
-  <si>
-    <t>%</t>
-  </si>
-  <si>
-    <t>DES2017</t>
-  </si>
-  <si>
-    <t>9/47</t>
-  </si>
-  <si>
-    <t>Unknown(47)</t>
-  </si>
-  <si>
-    <t>47/47</t>
-  </si>
-  <si>
-    <t>3/84</t>
-  </si>
-  <si>
-    <t>Unknown(84)</t>
-  </si>
-  <si>
-    <t>83/84</t>
-  </si>
-  <si>
-    <t>DES2017+Jacobs</t>
-  </si>
-  <si>
-    <t>21/131</t>
-  </si>
-  <si>
-    <t>Unknown(131)</t>
-  </si>
-  <si>
-    <t>241/256</t>
-  </si>
-  <si>
-    <t>X = Images</t>
-  </si>
-  <si>
-    <t>Y = Labels</t>
-  </si>
-  <si>
-    <t>Accuracy Rate</t>
-  </si>
-  <si>
-    <t>0.965</t>
-  </si>
-  <si>
     <t>clf_image = MLPClassifier(activation = 'relu',</t>
   </si>
   <si>
@@ -252,13 +99,28 @@
   </si>
   <si>
     <t>max_iter=100)</t>
+  </si>
+  <si>
+    <t>TEST 1</t>
+  </si>
+  <si>
+    <t>X = 20 000 Images</t>
+  </si>
+  <si>
+    <t>Y = 20 000 Labels(Gravitational Lense, Non Gravitational Lense)</t>
+  </si>
+  <si>
+    <t>Parameters</t>
+  </si>
+  <si>
+    <t>Data</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -274,19 +136,33 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Menlo"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="22">
     <border>
@@ -502,15 +378,6 @@
     </border>
     <border>
       <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -551,9 +418,22 @@
     </border>
     <border>
       <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right/>
       <top/>
-      <bottom style="medium">
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -564,7 +444,7 @@
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom style="medium">
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -573,9 +453,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
@@ -585,14 +464,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -605,13 +476,30 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -926,413 +814,216 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A06CD785-33B7-3045-A313-C2EB4D15E3B6}">
-  <dimension ref="A1:E38"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34:C38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.33203125" customWidth="1"/>
-    <col min="2" max="2" width="24.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="56.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="48.33203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="56.1640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.1640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="14"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="20"/>
-      <c r="B2" s="6" t="s">
+      <c r="A2" s="11"/>
+      <c r="B2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="21"/>
-      <c r="B4" s="9" t="s">
+      <c r="A4" s="12"/>
+      <c r="B4" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="9" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="22"/>
-      <c r="B5" s="6" t="s">
+    <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="13"/>
+      <c r="B5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="7" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="11"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
+      <c r="A6" s="15"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="11"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="23" t="s">
+      <c r="A7" s="15"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+    </row>
+    <row r="8" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="21"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="15"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C9" s="16"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="25" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="23"/>
-      <c r="B9" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="25"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="25"/>
+    </row>
+    <row r="13" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="27"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="C9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="23"/>
-      <c r="B10" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="23"/>
-      <c r="B11" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="23"/>
-      <c r="B12" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="23"/>
-      <c r="B13" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="23"/>
-      <c r="B14" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" t="s">
-        <v>30</v>
-      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="23"/>
-      <c r="B15" t="s">
-        <v>31</v>
-      </c>
-      <c r="C15" t="s">
-        <v>32</v>
-      </c>
+      <c r="A15" s="17"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="23"/>
-      <c r="B16" t="s">
-        <v>34</v>
-      </c>
-      <c r="C16" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="23"/>
-      <c r="B17" t="s">
-        <v>36</v>
-      </c>
-      <c r="C17" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="23"/>
-      <c r="B18" t="s">
-        <v>38</v>
-      </c>
-      <c r="C18" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="23"/>
-      <c r="B19" t="s">
-        <v>40</v>
-      </c>
-      <c r="C19" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="23"/>
-      <c r="B20" t="s">
-        <v>42</v>
-      </c>
-      <c r="C20" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="23"/>
-      <c r="B21" t="s">
-        <v>44</v>
-      </c>
-      <c r="C21" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="23"/>
-    </row>
-    <row r="23" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="24" t="s">
-        <v>46</v>
-      </c>
-      <c r="B23" s="24"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>48</v>
-      </c>
-      <c r="B26" t="s">
-        <v>49</v>
-      </c>
-      <c r="C26" t="s">
-        <v>50</v>
-      </c>
-      <c r="D26" t="s">
-        <v>51</v>
-      </c>
-      <c r="E26" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>53</v>
-      </c>
-      <c r="B27">
-        <v>9</v>
-      </c>
-      <c r="C27">
-        <v>38</v>
-      </c>
-      <c r="D27" t="s">
-        <v>54</v>
-      </c>
-      <c r="E27">
-        <f>(B27/47)*100</f>
-        <v>19.148936170212767</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>55</v>
-      </c>
-      <c r="B28">
-        <v>0</v>
-      </c>
-      <c r="C28">
-        <v>47</v>
-      </c>
-      <c r="D28" t="s">
-        <v>56</v>
-      </c>
-      <c r="E28">
-        <f>(C28/47)*100</f>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>33</v>
-      </c>
-      <c r="B29">
-        <v>3</v>
-      </c>
-      <c r="C29">
-        <v>81</v>
-      </c>
-      <c r="D29" t="s">
-        <v>57</v>
-      </c>
-      <c r="E29">
-        <f>(B29/84)*100</f>
-        <v>3.5714285714285712</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>58</v>
-      </c>
-      <c r="B30">
-        <v>1</v>
-      </c>
-      <c r="C30">
-        <v>83</v>
-      </c>
-      <c r="D30" t="s">
-        <v>59</v>
-      </c>
-      <c r="E30">
-        <f>(83/84)*100</f>
-        <v>98.80952380952381</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>60</v>
-      </c>
-      <c r="B31">
-        <v>21</v>
-      </c>
-      <c r="C31">
-        <v>110</v>
-      </c>
-      <c r="D31" t="s">
-        <v>61</v>
-      </c>
-      <c r="E31">
-        <f>(21/131)*100</f>
-        <v>16.030534351145036</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>62</v>
-      </c>
-      <c r="B32">
-        <v>15</v>
-      </c>
-      <c r="C32">
-        <v>241</v>
-      </c>
-      <c r="D32" t="s">
-        <v>63</v>
-      </c>
-      <c r="E32">
-        <f>(241/256)*100</f>
-        <v>94.140625</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+      <c r="A16" s="17"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="17"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="17"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="17"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="17"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="17"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="17"/>
+    </row>
+    <row r="23" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="18"/>
+      <c r="B23" s="18"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" s="15"/>
+      <c r="B32" s="15"/>
+      <c r="C32" s="15"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" s="15"/>
+      <c r="B33" s="15"/>
+      <c r="C33" s="15"/>
+    </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="B34" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="C34" s="14" t="s">
-        <v>68</v>
-      </c>
+      <c r="A34" s="15"/>
+      <c r="B34" s="15"/>
+      <c r="C34" s="19"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="B35" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="C35" s="16" t="s">
-        <v>69</v>
-      </c>
+      <c r="A35" s="15"/>
+      <c r="B35" s="15"/>
+      <c r="C35" s="19"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="15"/>
-      <c r="B36" s="11"/>
-      <c r="C36" s="16" t="s">
-        <v>70</v>
-      </c>
+      <c r="B36" s="15"/>
+      <c r="C36" s="19"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="15"/>
-      <c r="B37" s="11"/>
-      <c r="C37" s="16" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="17"/>
-      <c r="B38" s="18"/>
-      <c r="C38" s="25" t="s">
-        <v>72</v>
-      </c>
+      <c r="B37" s="15"/>
+      <c r="C37" s="19"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" s="15"/>
+      <c r="B38" s="15"/>
+      <c r="C38" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="A3:A5"/>
-    <mergeCell ref="A8:A22"/>
     <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A8:B8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>